<commit_message>
check appA + data format table + start intro
</commit_message>
<xml_diff>
--- a/documents/FONTANA_Tableau de proposition des rapporteurs & membres du jury.xlsx
+++ b/documents/FONTANA_Tableau de proposition des rapporteurs & membres du jury.xlsx
@@ -22,6 +22,7 @@
     <definedName name="_xlnm.Print_Area" localSheetId="2">'liste de choix'!$E$4:$E$21</definedName>
   </definedNames>
   <calcPr calcId="150001" concurrentCalc="0"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1212" uniqueCount="673">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1236" uniqueCount="673">
   <si>
     <t>N° ED 160 - Électronique, Électrotechnique, Automatique de Lyon (EEA)</t>
   </si>
@@ -5518,9 +5519,6 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="32" fillId="0" borderId="0" xfId="3"/>
-    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="29" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -5529,6 +5527,9 @@
     </xf>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="28" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -7273,8 +7274,8 @@
   </sheetPr>
   <dimension ref="A2:E278"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="89" workbookViewId="0">
-      <selection activeCell="C219" sqref="C219"/>
+    <sheetView tabSelected="1" topLeftCell="A2" zoomScale="89" zoomScaleNormal="89" zoomScalePageLayoutView="89" workbookViewId="0">
+      <selection activeCell="E149" sqref="E149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14" x14ac:dyDescent="0.15"/>
@@ -7666,16 +7667,16 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:5" ht="63.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="C2" s="108" t="s">
+      <c r="C2" s="111" t="s">
         <v>112</v>
       </c>
-      <c r="D2" s="108"/>
+      <c r="D2" s="111"/>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.15">
-      <c r="C3" s="111" t="s">
+      <c r="C3" s="110" t="s">
         <v>163</v>
       </c>
-      <c r="D3" s="111"/>
+      <c r="D3" s="110"/>
     </row>
     <row r="5" spans="1:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B5" s="1"/>
@@ -8250,8 +8251,8 @@
       <c r="B54" s="61" t="s">
         <v>499</v>
       </c>
-      <c r="C54" s="48" t="s">
-        <v>599</v>
+      <c r="C54" s="25" t="s">
+        <v>598</v>
       </c>
       <c r="D54" s="72" t="s">
         <v>493</v>
@@ -8265,7 +8266,7 @@
         <v>495</v>
       </c>
       <c r="C55" s="23" t="s">
-        <v>613</v>
+        <v>621</v>
       </c>
       <c r="D55" s="50" t="s">
         <v>463</v>
@@ -8279,7 +8280,7 @@
         <v>496</v>
       </c>
       <c r="C56" s="23" t="s">
-        <v>614</v>
+        <v>619</v>
       </c>
       <c r="D56" s="50" t="s">
         <v>464</v>
@@ -8292,8 +8293,8 @@
       <c r="B57" s="52" t="s">
         <v>497</v>
       </c>
-      <c r="C57" s="49" t="s">
-        <v>615</v>
+      <c r="C57" s="47" t="s">
+        <v>620</v>
       </c>
       <c r="D57" s="10"/>
     </row>
@@ -8307,7 +8308,7 @@
       <c r="C58" s="23" t="s">
         <v>442</v>
       </c>
-      <c r="D58" s="109" t="s">
+      <c r="D58" s="108" t="s">
         <v>546</v>
       </c>
     </row>
@@ -8315,8 +8316,8 @@
       <c r="B59" s="75" t="s">
         <v>498</v>
       </c>
-      <c r="C59" s="23"/>
-      <c r="D59" s="110"/>
+      <c r="C59" s="26"/>
+      <c r="D59" s="109"/>
     </row>
     <row r="60" spans="1:5" s="8" customFormat="1" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="8" t="s">
@@ -8340,7 +8341,7 @@
         <v>503</v>
       </c>
       <c r="C61" s="23" t="s">
-        <v>617</v>
+        <v>624</v>
       </c>
       <c r="D61" s="50" t="s">
         <v>505</v>
@@ -8354,7 +8355,7 @@
         <v>507</v>
       </c>
       <c r="C62" s="23" t="s">
-        <v>616</v>
+        <v>625</v>
       </c>
       <c r="D62" s="10" t="s">
         <v>504</v>
@@ -8392,7 +8393,7 @@
         <v>469</v>
       </c>
       <c r="C65" s="93" t="s">
-        <v>618</v>
+        <v>626</v>
       </c>
       <c r="D65" s="39"/>
     </row>
@@ -8404,7 +8405,7 @@
         <v>470</v>
       </c>
       <c r="C66" s="23" t="s">
-        <v>629</v>
+        <v>627</v>
       </c>
       <c r="D66" s="50" t="s">
         <v>466</v>
@@ -8418,7 +8419,7 @@
         <v>502</v>
       </c>
       <c r="C67" s="24" t="s">
-        <v>630</v>
+        <v>628</v>
       </c>
       <c r="D67" s="69" t="s">
         <v>467</v>
@@ -8444,8 +8445,8 @@
       <c r="B70" s="61" t="s">
         <v>499</v>
       </c>
-      <c r="C70" s="25" t="s">
-        <v>598</v>
+      <c r="C70" s="48" t="s">
+        <v>599</v>
       </c>
       <c r="D70" s="72" t="s">
         <v>493</v>
@@ -8459,7 +8460,7 @@
         <v>495</v>
       </c>
       <c r="C71" s="23" t="s">
-        <v>621</v>
+        <v>613</v>
       </c>
       <c r="D71" s="50" t="s">
         <v>463</v>
@@ -8473,7 +8474,7 @@
         <v>496</v>
       </c>
       <c r="C72" s="23" t="s">
-        <v>619</v>
+        <v>614</v>
       </c>
       <c r="D72" s="50" t="s">
         <v>464</v>
@@ -8486,8 +8487,8 @@
       <c r="B73" s="52" t="s">
         <v>515</v>
       </c>
-      <c r="C73" s="47" t="s">
-        <v>620</v>
+      <c r="C73" s="49" t="s">
+        <v>615</v>
       </c>
       <c r="D73" s="10"/>
     </row>
@@ -8501,7 +8502,7 @@
       <c r="C74" s="23" t="s">
         <v>442</v>
       </c>
-      <c r="D74" s="109" t="s">
+      <c r="D74" s="108" t="s">
         <v>547</v>
       </c>
     </row>
@@ -8509,8 +8510,8 @@
       <c r="B75" s="75" t="s">
         <v>498</v>
       </c>
-      <c r="C75" s="26"/>
-      <c r="D75" s="110"/>
+      <c r="C75" s="23"/>
+      <c r="D75" s="109"/>
     </row>
     <row r="76" spans="1:4" s="8" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A76" s="8" t="s">
@@ -8534,7 +8535,7 @@
         <v>510</v>
       </c>
       <c r="C77" s="23" t="s">
-        <v>624</v>
+        <v>617</v>
       </c>
       <c r="D77" s="50" t="s">
         <v>505</v>
@@ -8548,7 +8549,7 @@
         <v>507</v>
       </c>
       <c r="C78" s="23" t="s">
-        <v>625</v>
+        <v>616</v>
       </c>
       <c r="D78" s="10" t="s">
         <v>504</v>
@@ -8586,7 +8587,7 @@
         <v>469</v>
       </c>
       <c r="C81" s="93" t="s">
-        <v>626</v>
+        <v>618</v>
       </c>
       <c r="D81" s="39"/>
     </row>
@@ -8598,7 +8599,7 @@
         <v>470</v>
       </c>
       <c r="C82" s="23" t="s">
-        <v>627</v>
+        <v>629</v>
       </c>
       <c r="D82" s="50" t="s">
         <v>466</v>
@@ -8612,7 +8613,7 @@
         <v>502</v>
       </c>
       <c r="C83" s="24" t="s">
-        <v>628</v>
+        <v>630</v>
       </c>
       <c r="D83" s="69" t="s">
         <v>467</v>
@@ -8685,7 +8686,7 @@
         <v>511</v>
       </c>
       <c r="C90" s="23"/>
-      <c r="D90" s="109" t="s">
+      <c r="D90" s="108" t="s">
         <v>548</v>
       </c>
     </row>
@@ -8694,7 +8695,7 @@
         <v>498</v>
       </c>
       <c r="C91" s="26"/>
-      <c r="D91" s="110"/>
+      <c r="D91" s="109"/>
     </row>
     <row r="92" spans="1:4" s="8" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A92" s="8" t="s">
@@ -8835,7 +8836,7 @@
         <v>495</v>
       </c>
       <c r="C104" s="23" t="s">
-        <v>631</v>
+        <v>637</v>
       </c>
       <c r="D104" s="50" t="s">
         <v>463</v>
@@ -8849,7 +8850,7 @@
         <v>496</v>
       </c>
       <c r="C105" s="23" t="s">
-        <v>632</v>
+        <v>638</v>
       </c>
       <c r="D105" s="50" t="s">
         <v>464</v>
@@ -8865,7 +8866,7 @@
       <c r="C106" s="23" t="s">
         <v>122</v>
       </c>
-      <c r="D106" s="109" t="s">
+      <c r="D106" s="108" t="s">
         <v>549</v>
       </c>
     </row>
@@ -8874,7 +8875,7 @@
         <v>498</v>
       </c>
       <c r="C107" s="23"/>
-      <c r="D107" s="110"/>
+      <c r="D107" s="109"/>
     </row>
     <row r="108" spans="1:4" s="8" customFormat="1" ht="32.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A108" s="8" t="s">
@@ -8884,7 +8885,7 @@
         <v>453</v>
       </c>
       <c r="C108" s="23" t="s">
-        <v>451</v>
+        <v>109</v>
       </c>
       <c r="D108" s="76" t="s">
         <v>475</v>
@@ -8911,8 +8912,8 @@
       <c r="B110" s="52" t="s">
         <v>516</v>
       </c>
-      <c r="C110" s="47" t="s">
-        <v>643</v>
+      <c r="C110" s="49" t="s">
+        <v>657</v>
       </c>
       <c r="D110" s="39"/>
     </row>
@@ -8924,7 +8925,7 @@
         <v>517</v>
       </c>
       <c r="C111" s="23" t="s">
-        <v>644</v>
+        <v>660</v>
       </c>
       <c r="D111" s="50" t="s">
         <v>505</v>
@@ -8938,7 +8939,7 @@
         <v>507</v>
       </c>
       <c r="C112" s="23" t="s">
-        <v>645</v>
+        <v>658</v>
       </c>
       <c r="D112" s="10" t="s">
         <v>504</v>
@@ -8975,8 +8976,8 @@
       <c r="B115" s="52" t="s">
         <v>469</v>
       </c>
-      <c r="C115" s="93" t="s">
-        <v>646</v>
+      <c r="C115" s="23">
+        <v>69622</v>
       </c>
       <c r="D115" s="39"/>
     </row>
@@ -8988,7 +8989,7 @@
         <v>470</v>
       </c>
       <c r="C116" s="23" t="s">
-        <v>647</v>
+        <v>659</v>
       </c>
       <c r="D116" s="50" t="s">
         <v>466</v>
@@ -9002,7 +9003,7 @@
         <v>502</v>
       </c>
       <c r="C117" s="24" t="s">
-        <v>630</v>
+        <v>607</v>
       </c>
       <c r="D117" s="69" t="s">
         <v>467</v>
@@ -9044,7 +9045,7 @@
         <v>495</v>
       </c>
       <c r="C121" s="23" t="s">
-        <v>633</v>
+        <v>635</v>
       </c>
       <c r="D121" s="50" t="s">
         <v>463</v>
@@ -9058,7 +9059,7 @@
         <v>496</v>
       </c>
       <c r="C122" s="23" t="s">
-        <v>634</v>
+        <v>636</v>
       </c>
       <c r="D122" s="50" t="s">
         <v>464</v>
@@ -9072,9 +9073,9 @@
         <v>520</v>
       </c>
       <c r="C123" s="23" t="s">
-        <v>122</v>
-      </c>
-      <c r="D123" s="109" t="s">
+        <v>118</v>
+      </c>
+      <c r="D123" s="108" t="s">
         <v>550</v>
       </c>
     </row>
@@ -9083,7 +9084,7 @@
         <v>498</v>
       </c>
       <c r="C124" s="23"/>
-      <c r="D124" s="110"/>
+      <c r="D124" s="109"/>
     </row>
     <row r="125" spans="1:4" s="8" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A125" s="8" t="s">
@@ -9093,7 +9094,7 @@
         <v>453</v>
       </c>
       <c r="C125" s="23" t="s">
-        <v>109</v>
+        <v>451</v>
       </c>
       <c r="D125" s="76" t="s">
         <v>475</v>
@@ -9121,7 +9122,7 @@
         <v>518</v>
       </c>
       <c r="C127" s="49" t="s">
-        <v>648</v>
+        <v>653</v>
       </c>
       <c r="D127" s="39"/>
     </row>
@@ -9133,7 +9134,7 @@
         <v>519</v>
       </c>
       <c r="C128" s="23" t="s">
-        <v>649</v>
+        <v>654</v>
       </c>
       <c r="D128" s="50" t="s">
         <v>505</v>
@@ -9147,7 +9148,7 @@
         <v>507</v>
       </c>
       <c r="C129" s="23" t="s">
-        <v>650</v>
+        <v>655</v>
       </c>
       <c r="D129" s="10" t="s">
         <v>504</v>
@@ -9184,8 +9185,8 @@
       <c r="B132" s="52" t="s">
         <v>469</v>
       </c>
-      <c r="C132" s="93" t="s">
-        <v>651</v>
+      <c r="C132" s="23">
+        <v>10125</v>
       </c>
       <c r="D132" s="39"/>
     </row>
@@ -9197,7 +9198,7 @@
         <v>470</v>
       </c>
       <c r="C133" s="23" t="s">
-        <v>652</v>
+        <v>656</v>
       </c>
       <c r="D133" s="50" t="s">
         <v>466</v>
@@ -9211,7 +9212,7 @@
         <v>502</v>
       </c>
       <c r="C134" s="24" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="D134" s="69" t="s">
         <v>467</v>
@@ -9253,7 +9254,7 @@
         <v>495</v>
       </c>
       <c r="C138" s="23" t="s">
-        <v>635</v>
+        <v>641</v>
       </c>
       <c r="D138" s="50" t="s">
         <v>463</v>
@@ -9267,7 +9268,7 @@
         <v>496</v>
       </c>
       <c r="C139" s="23" t="s">
-        <v>636</v>
+        <v>642</v>
       </c>
       <c r="D139" s="50" t="s">
         <v>464</v>
@@ -9281,9 +9282,9 @@
         <v>521</v>
       </c>
       <c r="C140" s="23" t="s">
-        <v>118</v>
-      </c>
-      <c r="D140" s="109" t="s">
+        <v>120</v>
+      </c>
+      <c r="D140" s="108" t="s">
         <v>551</v>
       </c>
     </row>
@@ -9292,7 +9293,7 @@
         <v>498</v>
       </c>
       <c r="C141" s="23"/>
-      <c r="D141" s="110"/>
+      <c r="D141" s="109"/>
     </row>
     <row r="142" spans="1:4" s="8" customFormat="1" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A142" s="8" t="s">
@@ -9302,7 +9303,7 @@
         <v>453</v>
       </c>
       <c r="C142" s="23" t="s">
-        <v>451</v>
+        <v>109</v>
       </c>
       <c r="D142" s="76" t="s">
         <v>475</v>
@@ -9316,7 +9317,7 @@
         <v>376</v>
       </c>
       <c r="C143" s="23" t="s">
-        <v>150</v>
+        <v>146</v>
       </c>
       <c r="D143" s="76" t="s">
         <v>475</v>
@@ -9330,7 +9331,7 @@
         <v>522</v>
       </c>
       <c r="C144" s="49" t="s">
-        <v>653</v>
+        <v>612</v>
       </c>
       <c r="D144" s="39"/>
     </row>
@@ -9342,7 +9343,7 @@
         <v>523</v>
       </c>
       <c r="C145" s="23" t="s">
-        <v>654</v>
+        <v>662</v>
       </c>
       <c r="D145" s="50" t="s">
         <v>505</v>
@@ -9356,7 +9357,7 @@
         <v>507</v>
       </c>
       <c r="C146" s="23" t="s">
-        <v>655</v>
+        <v>664</v>
       </c>
       <c r="D146" s="10" t="s">
         <v>504</v>
@@ -9393,8 +9394,8 @@
       <c r="B149" s="52" t="s">
         <v>469</v>
       </c>
-      <c r="C149" s="23">
-        <v>10125</v>
+      <c r="C149" s="93" t="s">
+        <v>663</v>
       </c>
       <c r="D149" s="39"/>
     </row>
@@ -9406,7 +9407,7 @@
         <v>470</v>
       </c>
       <c r="C150" s="23" t="s">
-        <v>656</v>
+        <v>659</v>
       </c>
       <c r="D150" s="50" t="s">
         <v>466</v>
@@ -9420,7 +9421,7 @@
         <v>502</v>
       </c>
       <c r="C151" s="24" t="s">
-        <v>603</v>
+        <v>607</v>
       </c>
       <c r="D151" s="69" t="s">
         <v>467</v>
@@ -9462,7 +9463,7 @@
         <v>495</v>
       </c>
       <c r="C155" s="23" t="s">
-        <v>637</v>
+        <v>621</v>
       </c>
       <c r="D155" s="50" t="s">
         <v>463</v>
@@ -9476,7 +9477,7 @@
         <v>496</v>
       </c>
       <c r="C156" s="23" t="s">
-        <v>638</v>
+        <v>619</v>
       </c>
       <c r="D156" s="50" t="s">
         <v>464</v>
@@ -9490,9 +9491,9 @@
         <v>524</v>
       </c>
       <c r="C157" s="23" t="s">
-        <v>122</v>
-      </c>
-      <c r="D157" s="109" t="s">
+        <v>443</v>
+      </c>
+      <c r="D157" s="108" t="s">
         <v>552</v>
       </c>
     </row>
@@ -9501,7 +9502,7 @@
         <v>498</v>
       </c>
       <c r="C158" s="23"/>
-      <c r="D158" s="110"/>
+      <c r="D158" s="109"/>
     </row>
     <row r="159" spans="1:4" s="8" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A159" s="8" t="s">
@@ -9511,7 +9512,7 @@
         <v>453</v>
       </c>
       <c r="C159" s="23" t="s">
-        <v>109</v>
+        <v>451</v>
       </c>
       <c r="D159" s="76" t="s">
         <v>475</v>
@@ -9525,7 +9526,7 @@
         <v>377</v>
       </c>
       <c r="C160" s="23" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="D160" s="76" t="s">
         <v>475</v>
@@ -9538,8 +9539,8 @@
       <c r="B161" s="52" t="s">
         <v>525</v>
       </c>
-      <c r="C161" s="49" t="s">
-        <v>657</v>
+      <c r="C161" s="47" t="s">
+        <v>620</v>
       </c>
       <c r="D161" s="39"/>
     </row>
@@ -9551,7 +9552,7 @@
         <v>526</v>
       </c>
       <c r="C162" s="23" t="s">
-        <v>660</v>
+        <v>624</v>
       </c>
       <c r="D162" s="50" t="s">
         <v>505</v>
@@ -9565,7 +9566,7 @@
         <v>507</v>
       </c>
       <c r="C163" s="23" t="s">
-        <v>658</v>
+        <v>625</v>
       </c>
       <c r="D163" s="10" t="s">
         <v>504</v>
@@ -9602,8 +9603,8 @@
       <c r="B166" s="52" t="s">
         <v>469</v>
       </c>
-      <c r="C166" s="23">
-        <v>69622</v>
+      <c r="C166" s="93" t="s">
+        <v>626</v>
       </c>
       <c r="D166" s="39"/>
     </row>
@@ -9615,7 +9616,7 @@
         <v>470</v>
       </c>
       <c r="C167" s="23" t="s">
-        <v>659</v>
+        <v>627</v>
       </c>
       <c r="D167" s="50" t="s">
         <v>466</v>
@@ -9629,7 +9630,7 @@
         <v>502</v>
       </c>
       <c r="C168" s="24" t="s">
-        <v>607</v>
+        <v>628</v>
       </c>
       <c r="D168" s="69" t="s">
         <v>467</v>
@@ -9671,7 +9672,7 @@
         <v>495</v>
       </c>
       <c r="C172" s="23" t="s">
-        <v>639</v>
+        <v>633</v>
       </c>
       <c r="D172" s="50" t="s">
         <v>463</v>
@@ -9685,7 +9686,7 @@
         <v>496</v>
       </c>
       <c r="C173" s="23" t="s">
-        <v>640</v>
+        <v>634</v>
       </c>
       <c r="D173" s="50" t="s">
         <v>464</v>
@@ -9699,9 +9700,9 @@
         <v>527</v>
       </c>
       <c r="C174" s="23" t="s">
-        <v>120</v>
-      </c>
-      <c r="D174" s="109" t="s">
+        <v>122</v>
+      </c>
+      <c r="D174" s="108" t="s">
         <v>553</v>
       </c>
     </row>
@@ -9710,7 +9711,7 @@
         <v>498</v>
       </c>
       <c r="C175" s="23"/>
-      <c r="D175" s="110"/>
+      <c r="D175" s="109"/>
     </row>
     <row r="176" spans="1:4" s="8" customFormat="1" ht="33" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A176" s="8" t="s">
@@ -9734,7 +9735,7 @@
         <v>528</v>
       </c>
       <c r="C177" s="23" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="D177" s="76" t="s">
         <v>475</v>
@@ -9747,8 +9748,8 @@
       <c r="B178" s="52" t="s">
         <v>529</v>
       </c>
-      <c r="C178" s="47" t="s">
-        <v>610</v>
+      <c r="C178" s="49" t="s">
+        <v>648</v>
       </c>
       <c r="D178" s="39"/>
     </row>
@@ -9760,7 +9761,7 @@
         <v>530</v>
       </c>
       <c r="C179" s="23" t="s">
-        <v>660</v>
+        <v>649</v>
       </c>
       <c r="D179" s="50" t="s">
         <v>505</v>
@@ -9774,7 +9775,7 @@
         <v>507</v>
       </c>
       <c r="C180" s="23" t="s">
-        <v>658</v>
+        <v>650</v>
       </c>
       <c r="D180" s="10" t="s">
         <v>504</v>
@@ -9811,8 +9812,8 @@
       <c r="B183" s="52" t="s">
         <v>469</v>
       </c>
-      <c r="C183" s="23">
-        <v>69622</v>
+      <c r="C183" s="93" t="s">
+        <v>651</v>
       </c>
       <c r="D183" s="39"/>
     </row>
@@ -9824,7 +9825,7 @@
         <v>470</v>
       </c>
       <c r="C184" s="23" t="s">
-        <v>659</v>
+        <v>652</v>
       </c>
       <c r="D184" s="50" t="s">
         <v>466</v>
@@ -9866,7 +9867,7 @@
         <v>499</v>
       </c>
       <c r="C188" s="25" t="s">
-        <v>599</v>
+        <v>598</v>
       </c>
       <c r="D188" s="72" t="s">
         <v>493</v>
@@ -9880,7 +9881,7 @@
         <v>495</v>
       </c>
       <c r="C189" s="23" t="s">
-        <v>641</v>
+        <v>631</v>
       </c>
       <c r="D189" s="50" t="s">
         <v>463</v>
@@ -9894,7 +9895,7 @@
         <v>496</v>
       </c>
       <c r="C190" s="23" t="s">
-        <v>642</v>
+        <v>632</v>
       </c>
       <c r="D190" s="50" t="s">
         <v>464</v>
@@ -9908,9 +9909,9 @@
         <v>531</v>
       </c>
       <c r="C191" s="23" t="s">
-        <v>120</v>
-      </c>
-      <c r="D191" s="109" t="s">
+        <v>122</v>
+      </c>
+      <c r="D191" s="108" t="s">
         <v>554</v>
       </c>
     </row>
@@ -9919,7 +9920,7 @@
         <v>498</v>
       </c>
       <c r="C192" s="23"/>
-      <c r="D192" s="110"/>
+      <c r="D192" s="109"/>
     </row>
     <row r="193" spans="1:4" s="8" customFormat="1" ht="36" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A193" s="8" t="s">
@@ -9929,7 +9930,7 @@
         <v>453</v>
       </c>
       <c r="C193" s="23" t="s">
-        <v>109</v>
+        <v>451</v>
       </c>
       <c r="D193" s="76" t="s">
         <v>475</v>
@@ -9943,7 +9944,7 @@
         <v>532</v>
       </c>
       <c r="C194" s="23" t="s">
-        <v>146</v>
+        <v>150</v>
       </c>
       <c r="D194" s="76" t="s">
         <v>475</v>
@@ -9956,8 +9957,8 @@
       <c r="B195" s="52" t="s">
         <v>533</v>
       </c>
-      <c r="C195" s="49" t="s">
-        <v>612</v>
+      <c r="C195" s="47" t="s">
+        <v>643</v>
       </c>
       <c r="D195" s="39"/>
     </row>
@@ -9969,7 +9970,7 @@
         <v>534</v>
       </c>
       <c r="C196" s="23" t="s">
-        <v>662</v>
+        <v>644</v>
       </c>
       <c r="D196" s="50" t="s">
         <v>505</v>
@@ -9983,7 +9984,7 @@
         <v>507</v>
       </c>
       <c r="C197" s="23" t="s">
-        <v>664</v>
+        <v>645</v>
       </c>
       <c r="D197" s="10" t="s">
         <v>504</v>
@@ -10021,7 +10022,7 @@
         <v>469</v>
       </c>
       <c r="C200" s="93" t="s">
-        <v>663</v>
+        <v>646</v>
       </c>
       <c r="D200" s="39"/>
     </row>
@@ -10033,7 +10034,7 @@
         <v>470</v>
       </c>
       <c r="C201" s="23" t="s">
-        <v>659</v>
+        <v>647</v>
       </c>
       <c r="D201" s="50" t="s">
         <v>466</v>
@@ -10047,7 +10048,7 @@
         <v>502</v>
       </c>
       <c r="C202" s="24" t="s">
-        <v>607</v>
+        <v>630</v>
       </c>
       <c r="D202" s="69" t="s">
         <v>467</v>
@@ -10074,7 +10075,9 @@
       <c r="B205" s="61" t="s">
         <v>499</v>
       </c>
-      <c r="C205" s="48"/>
+      <c r="C205" s="25" t="s">
+        <v>599</v>
+      </c>
       <c r="D205" s="72" t="s">
         <v>493</v>
       </c>
@@ -10086,7 +10089,9 @@
       <c r="B206" s="52" t="s">
         <v>495</v>
       </c>
-      <c r="C206" s="23"/>
+      <c r="C206" s="23" t="s">
+        <v>639</v>
+      </c>
       <c r="D206" s="50" t="s">
         <v>463</v>
       </c>
@@ -10098,7 +10103,9 @@
       <c r="B207" s="52" t="s">
         <v>496</v>
       </c>
-      <c r="C207" s="23"/>
+      <c r="C207" s="23" t="s">
+        <v>640</v>
+      </c>
       <c r="D207" s="50" t="s">
         <v>464</v>
       </c>
@@ -10110,8 +10117,10 @@
       <c r="B208" s="52" t="s">
         <v>535</v>
       </c>
-      <c r="C208" s="23"/>
-      <c r="D208" s="109" t="s">
+      <c r="C208" s="23" t="s">
+        <v>120</v>
+      </c>
+      <c r="D208" s="108" t="s">
         <v>555</v>
       </c>
     </row>
@@ -10120,7 +10129,7 @@
         <v>498</v>
       </c>
       <c r="C209" s="23"/>
-      <c r="D209" s="110"/>
+      <c r="D209" s="109"/>
     </row>
     <row r="210" spans="1:4" s="8" customFormat="1" ht="34.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A210" s="8" t="s">
@@ -10129,7 +10138,9 @@
       <c r="B210" s="73" t="s">
         <v>453</v>
       </c>
-      <c r="C210" s="23"/>
+      <c r="C210" s="23" t="s">
+        <v>109</v>
+      </c>
       <c r="D210" s="76" t="s">
         <v>475</v>
       </c>
@@ -10141,7 +10152,9 @@
       <c r="B211" s="73" t="s">
         <v>536</v>
       </c>
-      <c r="C211" s="23"/>
+      <c r="C211" s="23" t="s">
+        <v>148</v>
+      </c>
       <c r="D211" s="76" t="s">
         <v>475</v>
       </c>
@@ -10153,7 +10166,9 @@
       <c r="B212" s="52" t="s">
         <v>537</v>
       </c>
-      <c r="C212" s="49"/>
+      <c r="C212" s="47" t="s">
+        <v>610</v>
+      </c>
       <c r="D212" s="39"/>
     </row>
     <row r="213" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -10163,7 +10178,9 @@
       <c r="B213" s="52" t="s">
         <v>538</v>
       </c>
-      <c r="C213" s="23"/>
+      <c r="C213" s="23" t="s">
+        <v>660</v>
+      </c>
       <c r="D213" s="50" t="s">
         <v>505</v>
       </c>
@@ -10175,7 +10192,9 @@
       <c r="B214" s="52" t="s">
         <v>507</v>
       </c>
-      <c r="C214" s="23"/>
+      <c r="C214" s="23" t="s">
+        <v>658</v>
+      </c>
       <c r="D214" s="10" t="s">
         <v>504</v>
       </c>
@@ -10211,7 +10230,9 @@
       <c r="B217" s="52" t="s">
         <v>469</v>
       </c>
-      <c r="C217" s="23"/>
+      <c r="C217" s="23">
+        <v>69622</v>
+      </c>
       <c r="D217" s="39"/>
     </row>
     <row r="218" spans="1:4" ht="34.5" customHeight="1" x14ac:dyDescent="0.15">
@@ -10221,7 +10242,9 @@
       <c r="B218" s="52" t="s">
         <v>470</v>
       </c>
-      <c r="C218" s="23"/>
+      <c r="C218" s="23" t="s">
+        <v>659</v>
+      </c>
       <c r="D218" s="50" t="s">
         <v>466</v>
       </c>
@@ -10233,7 +10256,9 @@
       <c r="B219" s="62" t="s">
         <v>502</v>
       </c>
-      <c r="C219" s="24"/>
+      <c r="C219" s="24" t="s">
+        <v>607</v>
+      </c>
       <c r="D219" s="69" t="s">
         <v>467</v>
       </c>
@@ -10259,7 +10284,9 @@
       <c r="B222" s="61" t="s">
         <v>499</v>
       </c>
-      <c r="C222" s="103"/>
+      <c r="C222" s="103" t="s">
+        <v>599</v>
+      </c>
       <c r="D222" s="72" t="s">
         <v>493</v>
       </c>
@@ -10271,7 +10298,9 @@
       <c r="B223" s="52" t="s">
         <v>495</v>
       </c>
-      <c r="C223" s="23"/>
+      <c r="C223" s="23" t="s">
+        <v>613</v>
+      </c>
       <c r="D223" s="50" t="s">
         <v>463</v>
       </c>
@@ -10283,7 +10312,9 @@
       <c r="B224" s="52" t="s">
         <v>496</v>
       </c>
-      <c r="C224" s="23"/>
+      <c r="C224" s="23" t="s">
+        <v>614</v>
+      </c>
       <c r="D224" s="50" t="s">
         <v>464</v>
       </c>
@@ -10295,8 +10326,10 @@
       <c r="B225" s="52" t="s">
         <v>541</v>
       </c>
-      <c r="C225" s="23"/>
-      <c r="D225" s="109" t="s">
+      <c r="C225" s="23" t="s">
+        <v>443</v>
+      </c>
+      <c r="D225" s="108" t="s">
         <v>556</v>
       </c>
     </row>
@@ -10305,7 +10338,7 @@
         <v>498</v>
       </c>
       <c r="C226" s="23"/>
-      <c r="D226" s="110"/>
+      <c r="D226" s="109"/>
     </row>
     <row r="227" spans="1:4" s="8" customFormat="1" ht="33.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A227" s="8" t="s">
@@ -10314,7 +10347,9 @@
       <c r="B227" s="73" t="s">
         <v>453</v>
       </c>
-      <c r="C227" s="23"/>
+      <c r="C227" s="23" t="s">
+        <v>451</v>
+      </c>
       <c r="D227" s="76" t="s">
         <v>475</v>
       </c>
@@ -10326,7 +10361,9 @@
       <c r="B228" s="73" t="s">
         <v>540</v>
       </c>
-      <c r="C228" s="23"/>
+      <c r="C228" s="23" t="s">
+        <v>152</v>
+      </c>
       <c r="D228" s="76" t="s">
         <v>475</v>
       </c>
@@ -10338,7 +10375,9 @@
       <c r="B229" s="52" t="s">
         <v>539</v>
       </c>
-      <c r="C229" s="23"/>
+      <c r="C229" s="49" t="s">
+        <v>615</v>
+      </c>
       <c r="D229" s="39"/>
     </row>
     <row r="230" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -10348,7 +10387,9 @@
       <c r="B230" s="52" t="s">
         <v>596</v>
       </c>
-      <c r="C230" s="23"/>
+      <c r="C230" s="23" t="s">
+        <v>617</v>
+      </c>
       <c r="D230" s="50" t="s">
         <v>505</v>
       </c>
@@ -10360,7 +10401,9 @@
       <c r="B231" s="52" t="s">
         <v>507</v>
       </c>
-      <c r="C231" s="23"/>
+      <c r="C231" s="23" t="s">
+        <v>616</v>
+      </c>
       <c r="D231" s="10" t="s">
         <v>504</v>
       </c>
@@ -10396,7 +10439,9 @@
       <c r="B234" s="52" t="s">
         <v>469</v>
       </c>
-      <c r="C234" s="23"/>
+      <c r="C234" s="93" t="s">
+        <v>618</v>
+      </c>
       <c r="D234" s="39"/>
     </row>
     <row r="235" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
@@ -10406,7 +10451,9 @@
       <c r="B235" s="52" t="s">
         <v>470</v>
       </c>
-      <c r="C235" s="23"/>
+      <c r="C235" s="23" t="s">
+        <v>629</v>
+      </c>
       <c r="D235" s="50" t="s">
         <v>466</v>
       </c>
@@ -10418,7 +10465,9 @@
       <c r="B236" s="62" t="s">
         <v>502</v>
       </c>
-      <c r="C236" s="24"/>
+      <c r="C236" s="24" t="s">
+        <v>630</v>
+      </c>
       <c r="D236" s="69" t="s">
         <v>467</v>
       </c>
@@ -10504,7 +10553,7 @@
       <c r="C244" s="23" t="s">
         <v>412</v>
       </c>
-      <c r="D244" s="109" t="s">
+      <c r="D244" s="108" t="s">
         <v>557</v>
       </c>
     </row>
@@ -10513,7 +10562,7 @@
         <v>498</v>
       </c>
       <c r="C245" s="23"/>
-      <c r="D245" s="110"/>
+      <c r="D245" s="109"/>
     </row>
     <row r="246" spans="1:4" ht="32.25" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A246" s="8" t="s">
@@ -10649,7 +10698,7 @@
         <v>545</v>
       </c>
       <c r="C257" s="23"/>
-      <c r="D257" s="109" t="s">
+      <c r="D257" s="108" t="s">
         <v>558</v>
       </c>
     </row>
@@ -10658,7 +10707,7 @@
         <v>498</v>
       </c>
       <c r="C258" s="23"/>
-      <c r="D258" s="110"/>
+      <c r="D258" s="109"/>
     </row>
     <row r="259" spans="1:4" ht="33.75" customHeight="1" x14ac:dyDescent="0.15">
       <c r="A259" s="8" t="s">
@@ -10870,11 +10919,6 @@
   <autoFilter ref="A6:A264"/>
   <dataConsolidate/>
   <mergeCells count="15">
-    <mergeCell ref="D208:D209"/>
-    <mergeCell ref="D225:D226"/>
-    <mergeCell ref="D244:D245"/>
-    <mergeCell ref="D257:D258"/>
-    <mergeCell ref="C3:D3"/>
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="D191:D192"/>
     <mergeCell ref="D74:D75"/>
@@ -10885,10 +10929,12 @@
     <mergeCell ref="D140:D141"/>
     <mergeCell ref="D174:D175"/>
     <mergeCell ref="D157:D158"/>
+    <mergeCell ref="D208:D209"/>
+    <mergeCell ref="D225:D226"/>
+    <mergeCell ref="D244:D245"/>
+    <mergeCell ref="D257:D258"/>
+    <mergeCell ref="C3:D3"/>
   </mergeCells>
-  <dataValidations xWindow="564" yWindow="602" count="1">
-    <dataValidation errorStyle="information" showInputMessage="1" showErrorMessage="1" errorTitle="ATTENTION" error="Votre saisie est différente des valeurs de la liste" sqref="C107"/>
-  </dataValidations>
   <hyperlinks>
     <hyperlink ref="C25" r:id="rId1"/>
     <hyperlink ref="C26" r:id="rId2"/>
@@ -10898,73 +10944,15 @@
     <hyperlink ref="C73" r:id="rId6"/>
     <hyperlink ref="C110" r:id="rId7"/>
     <hyperlink ref="C127" r:id="rId8"/>
-    <hyperlink ref="C144" r:id="rId9"/>
-    <hyperlink ref="C161" r:id="rId10"/>
-    <hyperlink ref="C178" r:id="rId11"/>
+    <hyperlink ref="C178" r:id="rId9"/>
+    <hyperlink ref="C195" r:id="rId10"/>
+    <hyperlink ref="C212" r:id="rId11"/>
+    <hyperlink ref="C229" r:id="rId12"/>
+    <hyperlink ref="C161" r:id="rId13"/>
   </hyperlinks>
   <pageMargins left="0.23622047244094491" right="0.23622047244094491" top="0.74803149606299213" bottom="0.74803149606299213" header="0.31496062992125984" footer="0.31496062992125984"/>
-  <pageSetup paperSize="8" scale="47" fitToHeight="4" orientation="portrait" r:id="rId12"/>
-  <drawing r:id="rId13"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xWindow="564" yWindow="602" count="9">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ERREUR" error="Votre saisie est différente des valeurs de la liste">
-          <x14:formula1>
-            <xm:f>'liste de choix'!$H$1:$H$7</xm:f>
-          </x14:formula1>
-          <xm:sqref>C143 C228 C194 C177 C160 C211 C126 C109</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ATTENTION" error="Votre saisie est différente des valeurs de la liste">
-          <x14:formula1>
-            <xm:f>'liste de choix'!$B$1:$B$91</xm:f>
-          </x14:formula1>
-          <xm:sqref>C42</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ATTENTION" error="Votre saisie est différente des valeurs de la liste">
-          <x14:formula1>
-            <xm:f>'liste de choix'!$E$1:$E$95</xm:f>
-          </x14:formula1>
-          <xm:sqref>C90 C257 C58 C74 C208 C225 C191 C157 C140 C123 C174 C244 C106</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>'liste de choix'!$F$1:$F$4</xm:f>
-          </x14:formula1>
-          <xm:sqref>C60 C76 C92 C125 C142 C210 C176 C193 C227 C159 C108</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ATTENTION" error="Votre saisie est différente des valeurs de la liste">
-          <x14:formula1>
-            <xm:f>'liste de choix'!$A$1:$A$2</xm:f>
-          </x14:formula1>
-          <xm:sqref>C222 C86 C70 C188 C154 C137 C171 C120 C254 C241 C54 C205 C103</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ERREUR" error="Votre saisie est différente des valeurs de la liste">
-          <x14:formula1>
-            <xm:f>'liste de choix'!$A$1:$A$2</xm:f>
-          </x14:formula1>
-          <xm:sqref>C9</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ATTENTION" error="Votre saisie est différente des valeurs de la liste">
-          <x14:formula1>
-            <xm:f>'liste de choix'!$D$1:$D$2</xm:f>
-          </x14:formula1>
-          <xm:sqref>C29 C39</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ATTENTION" error="Votre saisie est différente des valeurs de la liste">
-          <x14:formula1>
-            <xm:f>'liste de choix'!$I$1:$I$12</xm:f>
-          </x14:formula1>
-          <xm:sqref>C41</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="ATTENTION" error="Votre saisie est différente des valeurs de la liste">
-          <x14:formula1>
-            <xm:f>'liste de choix'!$C$1:$C$2</xm:f>
-          </x14:formula1>
-          <xm:sqref>C40</xm:sqref>
-        </x14:dataValidation>
-      </x14:dataValidations>
-    </ext>
-  </extLst>
+  <pageSetup paperSize="8" scale="47" fitToHeight="4" orientation="portrait" r:id="rId14"/>
+  <drawing r:id="rId15"/>
 </worksheet>
 </file>
 
@@ -11814,19 +11802,19 @@
       </c>
       <c r="AO2" t="str">
         <f>formulaire!C54</f>
-        <v>M.</v>
+        <v>Mme</v>
       </c>
       <c r="AP2" t="str">
         <f>formulaire!C55</f>
-        <v>THIROLF</v>
+        <v>LLOSÀ LLÁCER</v>
       </c>
       <c r="AQ2" t="str">
         <f>formulaire!C56</f>
-        <v>Peter</v>
+        <v>Gabriela</v>
       </c>
       <c r="AR2" t="str">
         <f>formulaire!C57</f>
-        <v>peter.thirolf@lmu.de</v>
+        <v>gabriela.llosa@ific.uv.es</v>
       </c>
       <c r="AS2" t="str">
         <f>formulaire!C58</f>
@@ -11838,11 +11826,11 @@
       </c>
       <c r="AU2" t="str">
         <f>formulaire!C61</f>
-        <v>Fakultät für Physik der LMU München - Lehrstuhl für Experimentalphysik - Medizinishce Physik</v>
+        <v>IFIC - Institut de Fisica Corpuscolar</v>
       </c>
       <c r="AV2" t="str">
         <f>formulaire!C62</f>
-        <v>Am Coulombwall 1</v>
+        <v>Parque Cuentufuco, C/Catedrático José Beltrán, 2</v>
       </c>
       <c r="AW2">
         <f>formulaire!C63</f>
@@ -11854,31 +11842,31 @@
       </c>
       <c r="AY2" t="str">
         <f>formulaire!C65</f>
-        <v xml:space="preserve">85748 </v>
+        <v>E-46980</v>
       </c>
       <c r="AZ2" t="str">
         <f>formulaire!C66</f>
-        <v>GARCHING</v>
+        <v>PATERNA</v>
       </c>
       <c r="BA2" t="str">
         <f>formulaire!C67</f>
-        <v>ALLEMAGNE</v>
+        <v>ESPAGNE</v>
       </c>
       <c r="BB2" t="str">
         <f>formulaire!C70</f>
-        <v>Mme</v>
+        <v>M.</v>
       </c>
       <c r="BC2" t="str">
         <f>formulaire!C71</f>
-        <v>LLOSÀ LLÁCER</v>
+        <v>THIROLF</v>
       </c>
       <c r="BD2" t="str">
         <f>formulaire!C72</f>
-        <v>Gabriela</v>
+        <v>Peter</v>
       </c>
       <c r="BE2" t="str">
         <f>formulaire!C73</f>
-        <v>gabriela.llosa@ific.uv.es</v>
+        <v>peter.thirolf@lmu.de</v>
       </c>
       <c r="BF2" t="str">
         <f>formulaire!C74</f>
@@ -11890,11 +11878,11 @@
       </c>
       <c r="BH2" t="str">
         <f>formulaire!C77</f>
-        <v>IFIC - Institut de Fisica Corpuscolar</v>
+        <v>Fakultät für Physik der LMU München - Lehrstuhl für Experimentalphysik - Medizinishce Physik</v>
       </c>
       <c r="BI2" t="str">
         <f>formulaire!C78</f>
-        <v>Parque Cuentufuco, C/Catedrático José Beltrán, 2</v>
+        <v>Am Coulombwall 1</v>
       </c>
       <c r="BJ2">
         <f>formulaire!C79</f>
@@ -11906,15 +11894,15 @@
       </c>
       <c r="BL2" t="str">
         <f>formulaire!C81</f>
-        <v>E-46980</v>
+        <v xml:space="preserve">85748 </v>
       </c>
       <c r="BM2" t="str">
         <f>formulaire!C82</f>
-        <v>PATERNA</v>
+        <v>GARCHING</v>
       </c>
       <c r="BN2" t="str">
         <f>formulaire!C83</f>
-        <v>ESPAGNE</v>
+        <v>ALLEMAGNE</v>
       </c>
       <c r="BO2">
         <f>formulaire!C86</f>
@@ -11974,11 +11962,11 @@
       </c>
       <c r="CC2" t="str">
         <f>formulaire!C104</f>
-        <v>RAFECAS</v>
+        <v>AUGIER</v>
       </c>
       <c r="CD2" t="str">
         <f>formulaire!C105</f>
-        <v>Magdalena</v>
+        <v>Corinne</v>
       </c>
       <c r="CE2" t="str">
         <f>formulaire!C106</f>
@@ -11986,7 +11974,7 @@
       </c>
       <c r="CF2" t="str">
         <f>formulaire!C108</f>
-        <v>équivalent</v>
+        <v>oui</v>
       </c>
       <c r="CG2" t="str">
         <f>formulaire!C109</f>
@@ -11994,15 +11982,15 @@
       </c>
       <c r="CH2" t="str">
         <f>formulaire!C110</f>
-        <v>rafecas@imt.uni.luebeck.de</v>
+        <v>c.augier@ipnl.in2p3.fr</v>
       </c>
       <c r="CI2" t="str">
         <f>formulaire!C111</f>
-        <v>Institut für Medizintechnik - Universität zu Lübeck</v>
+        <v>Institut de Physique Nucléaire de Lyon</v>
       </c>
       <c r="CJ2" t="str">
         <f>formulaire!C112</f>
-        <v>Ratzeburger Allee 160</v>
+        <v>4 Rue Enrico Fermi</v>
       </c>
       <c r="CK2">
         <f>formulaire!C113</f>
@@ -12012,17 +12000,17 @@
         <f>formulaire!C114</f>
         <v>0</v>
       </c>
-      <c r="CM2" t="str">
+      <c r="CM2">
         <f>formulaire!C115</f>
-        <v>23562</v>
+        <v>69622</v>
       </c>
       <c r="CN2" t="str">
         <f>formulaire!C116</f>
-        <v>LÜBECK</v>
+        <v>VILLEURBANNE</v>
       </c>
       <c r="CO2" t="str">
         <f>formulaire!C117</f>
-        <v>ALLEMAGNE</v>
+        <v>FRANCE</v>
       </c>
       <c r="CP2" t="str">
         <f>formulaire!C120</f>
@@ -12030,19 +12018,19 @@
       </c>
       <c r="CQ2" t="str">
         <f>formulaire!C121</f>
-        <v>MOREL</v>
+        <v>CERELLO</v>
       </c>
       <c r="CR2" t="str">
         <f>formulaire!C122</f>
-        <v>Christian</v>
+        <v>Piergiorgio</v>
       </c>
       <c r="CS2" t="str">
         <f>formulaire!C123</f>
-        <v>Professeur</v>
+        <v>Chercheur</v>
       </c>
       <c r="CT2" t="str">
         <f>formulaire!C125</f>
-        <v>oui</v>
+        <v>équivalent</v>
       </c>
       <c r="CU2" t="str">
         <f>formulaire!C126</f>
@@ -12050,15 +12038,15 @@
       </c>
       <c r="CV2" t="str">
         <f>formulaire!C127</f>
-        <v>morel@cppm.in2p3.fr</v>
+        <v>cerello@to.infn.it</v>
       </c>
       <c r="CW2" t="str">
         <f>formulaire!C128</f>
-        <v>Centre de Physique de Particules de Marseille - Aix-Marseille Université</v>
+        <v>Istituto Nazionale di Fisica Nucleare - Sezione di Torino</v>
       </c>
       <c r="CX2" t="str">
         <f>formulaire!C129</f>
-        <v>163 Avenue de Luminy</v>
+        <v>Via Pietro Giuria 1</v>
       </c>
       <c r="CY2">
         <f>formulaire!C130</f>
@@ -12068,17 +12056,17 @@
         <f>formulaire!C131</f>
         <v>0</v>
       </c>
-      <c r="DA2" t="str">
+      <c r="DA2">
         <f>formulaire!C132</f>
-        <v>13288 CEDEX 09</v>
+        <v>10125</v>
       </c>
       <c r="DB2" t="str">
         <f>formulaire!C133</f>
-        <v>MARSEILLE</v>
+        <v>TORINO</v>
       </c>
       <c r="DC2" t="str">
         <f>formulaire!C134</f>
-        <v>FRANCE</v>
+        <v>ITALIE</v>
       </c>
       <c r="DD2" t="str">
         <f>formulaire!C137</f>
@@ -12086,35 +12074,35 @@
       </c>
       <c r="DE2" t="str">
         <f>formulaire!C138</f>
-        <v>CERELLO</v>
+        <v>LÉTANG</v>
       </c>
       <c r="DF2" t="str">
         <f>formulaire!C139</f>
-        <v>Piergiorgio</v>
+        <v>Jean Michel</v>
       </c>
       <c r="DG2" t="str">
         <f>formulaire!C140</f>
-        <v>Chercheur</v>
+        <v>Maître de Conférences</v>
       </c>
       <c r="DH2" t="str">
         <f>formulaire!C142</f>
-        <v>équivalent</v>
+        <v>oui</v>
       </c>
       <c r="DI2" t="str">
         <f>formulaire!C143</f>
-        <v>Examinateur</v>
+        <v xml:space="preserve">Co-Directeur de thèse </v>
       </c>
       <c r="DJ2" t="str">
         <f>formulaire!C144</f>
-        <v>cerello@to.infn.it</v>
+        <v>jean-michel.letang@creatis.insa-lyon.fr</v>
       </c>
       <c r="DK2" t="str">
         <f>formulaire!C145</f>
-        <v>Istituto Nazionale di Fisica Nucleare - Sezione di Torino</v>
+        <v>CREATIS</v>
       </c>
       <c r="DL2" t="str">
         <f>formulaire!C146</f>
-        <v>Via Pietro Giuria 1</v>
+        <v>7 Avenue Jean Chapelle O</v>
       </c>
       <c r="DM2">
         <f>formulaire!C147</f>
@@ -12124,17 +12112,17 @@
         <f>formulaire!C148</f>
         <v>0</v>
       </c>
-      <c r="DO2">
+      <c r="DO2" t="str">
         <f>formulaire!C149</f>
-        <v>10125</v>
+        <v>69622</v>
       </c>
       <c r="DP2" t="str">
         <f>formulaire!C150</f>
-        <v>TORINO</v>
+        <v>VILLEURBANNE</v>
       </c>
       <c r="DQ2" t="str">
         <f>formulaire!C151</f>
-        <v>ITALIE</v>
+        <v>FRANCE</v>
       </c>
       <c r="DR2" t="str">
         <f>formulaire!C154</f>
@@ -12142,35 +12130,35 @@
       </c>
       <c r="DS2" t="str">
         <f>formulaire!C155</f>
-        <v>AUGIER</v>
+        <v>LLOSÀ LLÁCER</v>
       </c>
       <c r="DT2" t="str">
         <f>formulaire!C156</f>
-        <v>Corinne</v>
+        <v>Gabriela</v>
       </c>
       <c r="DU2" t="str">
         <f>formulaire!C157</f>
-        <v>Professeur</v>
+        <v>Professeure Associée</v>
       </c>
       <c r="DV2" t="str">
         <f>formulaire!C159</f>
-        <v>oui</v>
+        <v>équivalent</v>
       </c>
       <c r="DW2" t="str">
         <f>formulaire!C160</f>
-        <v>Examinateur</v>
+        <v>Rapporteur</v>
       </c>
       <c r="DX2" t="str">
         <f>formulaire!C161</f>
-        <v>c.augier@ipnl.in2p3.fr</v>
+        <v>gabriela.llosa@ific.uv.es</v>
       </c>
       <c r="DY2" t="str">
         <f>formulaire!C162</f>
-        <v>Institut de Physique Nucléaire de Lyon</v>
+        <v>IFIC - Institut de Fisica Corpuscolar</v>
       </c>
       <c r="DZ2" t="str">
         <f>formulaire!C163</f>
-        <v>4 Rue Enrico Fermi</v>
+        <v>Parque Cuentufuco, C/Catedrático José Beltrán, 2</v>
       </c>
       <c r="EA2">
         <f>formulaire!C164</f>
@@ -12180,17 +12168,17 @@
         <f>formulaire!C165</f>
         <v>0</v>
       </c>
-      <c r="EC2">
+      <c r="EC2" t="str">
         <f>formulaire!C166</f>
-        <v>69622</v>
+        <v>E-46980</v>
       </c>
       <c r="ED2" t="str">
         <f>formulaire!C167</f>
-        <v>VILLEURBANNE</v>
+        <v>PATERNA</v>
       </c>
       <c r="EE2" t="str">
         <f>formulaire!C168</f>
-        <v>FRANCE</v>
+        <v>ESPAGNE</v>
       </c>
       <c r="EF2" t="str">
         <f>formulaire!C171</f>
@@ -12198,15 +12186,15 @@
       </c>
       <c r="EG2" t="str">
         <f>formulaire!C172</f>
-        <v>TESTA</v>
+        <v>MOREL</v>
       </c>
       <c r="EH2" t="str">
         <f>formulaire!C173</f>
-        <v>Étienne</v>
+        <v>Christian</v>
       </c>
       <c r="EI2" t="str">
         <f>formulaire!C174</f>
-        <v>Maître de Conférences</v>
+        <v>Professeur</v>
       </c>
       <c r="EJ2" t="str">
         <f>formulaire!C176</f>
@@ -12214,19 +12202,19 @@
       </c>
       <c r="EK2" t="str">
         <f>formulaire!C177</f>
-        <v xml:space="preserve">Directeur de thèse </v>
+        <v>Examinateur</v>
       </c>
       <c r="EL2" t="str">
         <f>formulaire!C178</f>
-        <v>e.testa@ipnl.in2p3.fr</v>
+        <v>morel@cppm.in2p3.fr</v>
       </c>
       <c r="EM2" t="str">
         <f>formulaire!C179</f>
-        <v>Institut de Physique Nucléaire de Lyon</v>
+        <v>Centre de Physique de Particules de Marseille - Aix-Marseille Université</v>
       </c>
       <c r="EN2" t="str">
         <f>formulaire!C180</f>
-        <v>4 Rue Enrico Fermi</v>
+        <v>163 Avenue de Luminy</v>
       </c>
       <c r="EO2">
         <f>formulaire!C181</f>
@@ -12236,13 +12224,13 @@
         <f>formulaire!C182</f>
         <v>0</v>
       </c>
-      <c r="EQ2">
+      <c r="EQ2" t="str">
         <f>formulaire!C183</f>
-        <v>69622</v>
+        <v>13288 CEDEX 09</v>
       </c>
       <c r="ER2" t="str">
         <f>formulaire!C184</f>
-        <v>VILLEURBANNE</v>
+        <v>MARSEILLE</v>
       </c>
       <c r="ES2" t="str">
         <f>formulaire!C185</f>
@@ -12250,39 +12238,39 @@
       </c>
       <c r="ET2" t="str">
         <f>formulaire!C188</f>
-        <v>M.</v>
+        <v>Mme</v>
       </c>
       <c r="EU2" t="str">
         <f>formulaire!C189</f>
-        <v>LÉTANG</v>
+        <v>RAFECAS</v>
       </c>
       <c r="EV2" t="str">
         <f>formulaire!C190</f>
-        <v>Jean Michel</v>
+        <v>Magdalena</v>
       </c>
       <c r="EW2" t="str">
         <f>formulaire!C191</f>
-        <v>Maître de Conférences</v>
+        <v>Professeur</v>
       </c>
       <c r="EX2" t="str">
         <f>formulaire!C193</f>
-        <v>oui</v>
+        <v>équivalent</v>
       </c>
       <c r="EY2" t="str">
         <f>formulaire!C194</f>
-        <v xml:space="preserve">Co-Directeur de thèse </v>
+        <v>Examinateur</v>
       </c>
       <c r="EZ2" t="str">
         <f>formulaire!C195</f>
-        <v>jean-michel.letang@creatis.insa-lyon.fr</v>
+        <v>rafecas@imt.uni.luebeck.de</v>
       </c>
       <c r="FA2" t="str">
         <f>formulaire!C196</f>
-        <v>CREATIS</v>
+        <v>Institut für Medizintechnik - Universität zu Lübeck</v>
       </c>
       <c r="FB2" t="str">
         <f>formulaire!C197</f>
-        <v>7 Avenue Jean Chapelle O</v>
+        <v>Ratzeburger Allee 160</v>
       </c>
       <c r="FC2">
         <f>formulaire!C198</f>
@@ -12294,51 +12282,51 @@
       </c>
       <c r="FE2" t="str">
         <f>formulaire!C200</f>
-        <v>69622</v>
+        <v>23562</v>
       </c>
       <c r="FF2" t="str">
         <f>formulaire!C201</f>
-        <v>VILLEURBANNE</v>
+        <v>LÜBECK</v>
       </c>
       <c r="FG2" t="str">
         <f>formulaire!C202</f>
-        <v>FRANCE</v>
-      </c>
-      <c r="FH2">
+        <v>ALLEMAGNE</v>
+      </c>
+      <c r="FH2" t="str">
         <f>formulaire!C205</f>
-        <v>0</v>
-      </c>
-      <c r="FI2">
+        <v>M.</v>
+      </c>
+      <c r="FI2" t="str">
         <f>formulaire!C206</f>
-        <v>0</v>
-      </c>
-      <c r="FJ2">
+        <v>TESTA</v>
+      </c>
+      <c r="FJ2" t="str">
         <f>formulaire!C207</f>
-        <v>0</v>
-      </c>
-      <c r="FK2">
+        <v>Étienne</v>
+      </c>
+      <c r="FK2" t="str">
         <f>formulaire!C208</f>
-        <v>0</v>
-      </c>
-      <c r="FL2">
+        <v>Maître de Conférences</v>
+      </c>
+      <c r="FL2" t="str">
         <f>formulaire!C210</f>
-        <v>0</v>
-      </c>
-      <c r="FM2">
+        <v>oui</v>
+      </c>
+      <c r="FM2" t="str">
         <f>formulaire!C211</f>
-        <v>0</v>
-      </c>
-      <c r="FN2">
+        <v xml:space="preserve">Directeur de thèse </v>
+      </c>
+      <c r="FN2" t="str">
         <f>formulaire!C212</f>
-        <v>0</v>
-      </c>
-      <c r="FO2">
+        <v>e.testa@ipnl.in2p3.fr</v>
+      </c>
+      <c r="FO2" t="str">
         <f>formulaire!C213</f>
-        <v>0</v>
-      </c>
-      <c r="FP2">
+        <v>Institut de Physique Nucléaire de Lyon</v>
+      </c>
+      <c r="FP2" t="str">
         <f>formulaire!C214</f>
-        <v>0</v>
+        <v>4 Rue Enrico Fermi</v>
       </c>
       <c r="FQ2">
         <f>formulaire!C215</f>
@@ -12350,51 +12338,51 @@
       </c>
       <c r="FS2">
         <f>formulaire!C217</f>
-        <v>0</v>
-      </c>
-      <c r="FT2">
+        <v>69622</v>
+      </c>
+      <c r="FT2" t="str">
         <f>formulaire!C218</f>
-        <v>0</v>
-      </c>
-      <c r="FU2">
+        <v>VILLEURBANNE</v>
+      </c>
+      <c r="FU2" t="str">
         <f>formulaire!C219</f>
-        <v>0</v>
-      </c>
-      <c r="FV2">
+        <v>FRANCE</v>
+      </c>
+      <c r="FV2" t="str">
         <f>formulaire!C222</f>
-        <v>0</v>
-      </c>
-      <c r="FW2">
+        <v>M.</v>
+      </c>
+      <c r="FW2" t="str">
         <f>formulaire!C223</f>
-        <v>0</v>
-      </c>
-      <c r="FX2">
+        <v>THIROLF</v>
+      </c>
+      <c r="FX2" t="str">
         <f>formulaire!C224</f>
-        <v>0</v>
-      </c>
-      <c r="FY2">
+        <v>Peter</v>
+      </c>
+      <c r="FY2" t="str">
         <f>formulaire!C225</f>
-        <v>0</v>
-      </c>
-      <c r="FZ2">
+        <v>Professeure Associée</v>
+      </c>
+      <c r="FZ2" t="str">
         <f>formulaire!C227</f>
-        <v>0</v>
-      </c>
-      <c r="GA2">
+        <v>équivalent</v>
+      </c>
+      <c r="GA2" t="str">
         <f>formulaire!C228</f>
-        <v>0</v>
-      </c>
-      <c r="GB2">
+        <v>Rapporteur</v>
+      </c>
+      <c r="GB2" t="str">
         <f>formulaire!C229</f>
-        <v>0</v>
-      </c>
-      <c r="GC2">
+        <v>peter.thirolf@lmu.de</v>
+      </c>
+      <c r="GC2" t="str">
         <f>formulaire!C230</f>
-        <v>0</v>
-      </c>
-      <c r="GD2">
+        <v>Fakultät für Physik der LMU München - Lehrstuhl für Experimentalphysik - Medizinishce Physik</v>
+      </c>
+      <c r="GD2" t="str">
         <f>formulaire!C231</f>
-        <v>0</v>
+        <v>Am Coulombwall 1</v>
       </c>
       <c r="GE2">
         <f>formulaire!C232</f>
@@ -12404,17 +12392,17 @@
         <f>formulaire!C233</f>
         <v>0</v>
       </c>
-      <c r="GG2">
+      <c r="GG2" t="str">
         <f>formulaire!C234</f>
-        <v>0</v>
-      </c>
-      <c r="GH2">
+        <v xml:space="preserve">85748 </v>
+      </c>
+      <c r="GH2" t="str">
         <f>formulaire!C235</f>
-        <v>0</v>
-      </c>
-      <c r="GI2">
+        <v>GARCHING</v>
+      </c>
+      <c r="GI2" t="str">
         <f>formulaire!C236</f>
-        <v>0</v>
+        <v>ALLEMAGNE</v>
       </c>
       <c r="GJ2" t="str">
         <f>formulaire!C241</f>

</xml_diff>